<commit_message>
added 5th run data
</commit_message>
<xml_diff>
--- a/Results/ScenarioI-Proto-I/ScenarioI-ProtoI.xlsx
+++ b/Results/ScenarioI-Proto-I/ScenarioI-ProtoI.xlsx
@@ -402,7 +402,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,6 +1117,18 @@
       <c r="C39">
         <v>2</v>
       </c>
+      <c r="D39">
+        <v>1178.72</v>
+      </c>
+      <c r="E39">
+        <v>1178.72</v>
+      </c>
+      <c r="F39">
+        <v>1091.44</v>
+      </c>
+      <c r="G39">
+        <v>1040.1099999999999</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
@@ -1127,6 +1139,18 @@
       </c>
       <c r="C40">
         <v>2</v>
+      </c>
+      <c r="D40">
+        <v>1209.92</v>
+      </c>
+      <c r="E40">
+        <v>1209.92</v>
+      </c>
+      <c r="F40">
+        <v>1123.56</v>
+      </c>
+      <c r="G40">
+        <v>1058.18</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1139,6 +1163,18 @@
       <c r="C41">
         <v>2</v>
       </c>
+      <c r="D41">
+        <v>1195.1300000000001</v>
+      </c>
+      <c r="E41">
+        <v>1195.1300000000001</v>
+      </c>
+      <c r="F41">
+        <v>1109.03</v>
+      </c>
+      <c r="G41">
+        <v>1054.07</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
@@ -1149,6 +1185,18 @@
       </c>
       <c r="C42">
         <v>2</v>
+      </c>
+      <c r="D42">
+        <v>1226.33</v>
+      </c>
+      <c r="E42">
+        <v>1226.33</v>
+      </c>
+      <c r="F42">
+        <v>1140.1400000000001</v>
+      </c>
+      <c r="G42">
+        <v>1067.75</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1160,6 +1208,18 @@
       </c>
       <c r="C43">
         <v>2</v>
+      </c>
+      <c r="D43">
+        <v>1189.72</v>
+      </c>
+      <c r="E43">
+        <v>1189.72</v>
+      </c>
+      <c r="F43">
+        <v>1103.27</v>
+      </c>
+      <c r="G43">
+        <v>1041.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>